<commit_message>
session summary uses last trial settings
</commit_message>
<xml_diff>
--- a/BpodInfoseekLog.xlsx
+++ b/BpodInfoseekLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="5520" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="5520" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="JB366" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="230">
   <si>
     <t>'JB366_Infoseek_20201021_101114.mat'</t>
   </si>
@@ -716,6 +716,12 @@
   <si>
     <t>'JB373_Infoseek_20201113_134114.mat'</t>
   </si>
+  <si>
+    <t>'JB371_Infoseek_20201116_142113.mat'</t>
+  </si>
+  <si>
+    <t>'20201116'</t>
+  </si>
 </sst>
 </file>
 
@@ -19251,7 +19257,7 @@
   <dimension ref="A1:BM20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20953,10 +20959,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BM20"/>
+  <dimension ref="A1:BM19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21167,11 +21173,11 @@
       </c>
       <c r="BL1" s="10">
         <f>SUM($AN$2:$AN$1048576,$AP$2:$AP$1048576)</f>
-        <v>616</v>
+        <v>725</v>
       </c>
       <c r="BM1" s="10">
         <f>SUM($AO$2:$AO$1048576,$AQ$2:$AQ$1048576)</f>
-        <v>615</v>
+        <v>726</v>
       </c>
     </row>
     <row r="2" spans="1:65" s="22" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -21906,43 +21912,43 @@
         <v>193</v>
       </c>
       <c r="AZ5" s="12">
-        <f t="shared" ref="AZ5:AZ11" si="2">SUMIF($B$2:$B$1048576,$B5,$AE$2:$AE$1048576)</f>
+        <f>SUMIF($B$2:$B$1048576,$B5,$AE$2:$AE$1048576)</f>
         <v>284</v>
       </c>
       <c r="BA5" s="12">
-        <f t="shared" ref="BA5:BA11" si="3">SUMIF($B$2:$B$1048576,$B5,$AV$2:$AV$1048576)</f>
+        <f>SUMIF($B$2:$B$1048576,$B5,$AV$2:$AV$1048576)</f>
         <v>1116</v>
       </c>
       <c r="BB5" s="12">
-        <f t="shared" ref="BB5:BB11" si="4">SUMIF($B$2:$B$1048576,$B5,$AF$2:$AF$1048576)*60</f>
+        <f>SUMIF($B$2:$B$1048576,$B5,$AF$2:$AF$1048576)*60</f>
         <v>1835.5716999999977</v>
       </c>
       <c r="BC5" s="12">
-        <f t="shared" ref="BC5:BC7" si="5">BB5/AZ5</f>
+        <f t="shared" ref="BC5:BC7" si="2">BB5/AZ5</f>
         <v>6.4632806338028086</v>
       </c>
       <c r="BD5" s="12">
-        <f t="shared" ref="BD5:BD11" si="6">SUMIF($B$2:$B$1048576,$B5,$AN$2:$AN$1048576)</f>
+        <f>SUMIF($B$2:$B$1048576,$B5,$AN$2:$AN$1048576)</f>
         <v>156</v>
       </c>
       <c r="BE5" s="12">
-        <f t="shared" ref="BE5:BE11" si="7">SUMIF($B$2:$B$1048576,$B5,$AO$2:$AO$1048576)</f>
+        <f>SUMIF($B$2:$B$1048576,$B5,$AO$2:$AO$1048576)</f>
         <v>123</v>
       </c>
       <c r="BF5" s="12">
-        <f t="shared" ref="BF5:BF11" si="8">SUMIF($B$2:$B$1048576,$B5,$AP$2:$AP$1048576)</f>
+        <f>SUMIF($B$2:$B$1048576,$B5,$AP$2:$AP$1048576)</f>
         <v>0</v>
       </c>
       <c r="BG5" s="12">
-        <f t="shared" ref="BG5:BG11" si="9">SUMIF($B$2:$B$1048576,$B5,$AQ$2:$AQ$1048576)</f>
+        <f>SUMIF($B$2:$B$1048576,$B5,$AQ$2:$AQ$1048576)</f>
         <v>0</v>
       </c>
       <c r="BH5" s="1">
-        <f t="shared" ref="BH5:BH7" si="10">SUM(BD5,BF5)</f>
+        <f t="shared" ref="BH5:BH7" si="3">SUM(BD5,BF5)</f>
         <v>156</v>
       </c>
       <c r="BI5" s="1">
-        <f t="shared" ref="BI5:BI7" si="11">SUM(BE5,BG5)</f>
+        <f t="shared" ref="BI5:BI7" si="4">SUM(BE5,BG5)</f>
         <v>123</v>
       </c>
     </row>
@@ -22099,43 +22105,43 @@
         <v>193</v>
       </c>
       <c r="AZ6" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B6,$AE$2:$AE$1048576)</f>
+        <v>284</v>
+      </c>
+      <c r="BA6" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B6,$AV$2:$AV$1048576)</f>
+        <v>1116</v>
+      </c>
+      <c r="BB6" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B6,$AF$2:$AF$1048576)*60</f>
+        <v>1835.5716999999977</v>
+      </c>
+      <c r="BC6" s="12">
         <f t="shared" si="2"/>
-        <v>284</v>
-      </c>
-      <c r="BA6" s="12">
+        <v>6.4632806338028086</v>
+      </c>
+      <c r="BD6" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B6,$AN$2:$AN$1048576)</f>
+        <v>156</v>
+      </c>
+      <c r="BE6" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B6,$AO$2:$AO$1048576)</f>
+        <v>123</v>
+      </c>
+      <c r="BF6" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B6,$AP$2:$AP$1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="BG6" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B6,$AQ$2:$AQ$1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="BH6" s="1">
         <f t="shared" si="3"/>
-        <v>1116</v>
-      </c>
-      <c r="BB6" s="12">
+        <v>156</v>
+      </c>
+      <c r="BI6" s="1">
         <f t="shared" si="4"/>
-        <v>1835.5716999999977</v>
-      </c>
-      <c r="BC6" s="12">
-        <f t="shared" si="5"/>
-        <v>6.4632806338028086</v>
-      </c>
-      <c r="BD6" s="12">
-        <f t="shared" si="6"/>
-        <v>156</v>
-      </c>
-      <c r="BE6" s="12">
-        <f t="shared" si="7"/>
-        <v>123</v>
-      </c>
-      <c r="BF6" s="12">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="BG6" s="12">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BH6" s="1">
-        <f t="shared" si="10"/>
-        <v>156</v>
-      </c>
-      <c r="BI6" s="1">
-        <f t="shared" si="11"/>
         <v>123</v>
       </c>
     </row>
@@ -22292,43 +22298,43 @@
         <v>193</v>
       </c>
       <c r="AZ7" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B7,$AE$2:$AE$1048576)</f>
+        <v>284</v>
+      </c>
+      <c r="BA7" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B7,$AV$2:$AV$1048576)</f>
+        <v>1116</v>
+      </c>
+      <c r="BB7" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B7,$AF$2:$AF$1048576)*60</f>
+        <v>1835.5716999999977</v>
+      </c>
+      <c r="BC7" s="10">
         <f t="shared" si="2"/>
-        <v>284</v>
-      </c>
-      <c r="BA7" s="10">
+        <v>6.4632806338028086</v>
+      </c>
+      <c r="BD7" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B7,$AN$2:$AN$1048576)</f>
+        <v>156</v>
+      </c>
+      <c r="BE7" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B7,$AO$2:$AO$1048576)</f>
+        <v>123</v>
+      </c>
+      <c r="BF7" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B7,$AP$2:$AP$1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="BG7" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B7,$AQ$2:$AQ$1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="BH7" s="22">
         <f t="shared" si="3"/>
-        <v>1116</v>
-      </c>
-      <c r="BB7" s="10">
+        <v>156</v>
+      </c>
+      <c r="BI7" s="22">
         <f t="shared" si="4"/>
-        <v>1835.5716999999977</v>
-      </c>
-      <c r="BC7" s="10">
-        <f t="shared" si="5"/>
-        <v>6.4632806338028086</v>
-      </c>
-      <c r="BD7" s="10">
-        <f t="shared" si="6"/>
-        <v>156</v>
-      </c>
-      <c r="BE7" s="10">
-        <f t="shared" si="7"/>
-        <v>123</v>
-      </c>
-      <c r="BF7" s="10">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="BG7" s="10">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BH7" s="22">
-        <f t="shared" si="10"/>
-        <v>156</v>
-      </c>
-      <c r="BI7" s="22">
-        <f t="shared" si="11"/>
         <v>123</v>
       </c>
     </row>
@@ -22478,50 +22484,50 @@
         <v>764</v>
       </c>
       <c r="AX8" s="22" t="str">
-        <f t="shared" ref="AX8:AX10" si="12">B8</f>
+        <f t="shared" ref="AX8:AX10" si="5">B8</f>
         <v>'20201112'</v>
       </c>
       <c r="AY8" s="26" t="s">
         <v>193</v>
       </c>
       <c r="AZ8" s="10">
-        <f t="shared" si="2"/>
+        <f>SUMIF($B$2:$B$1048576,$B8,$AE$2:$AE$1048576)</f>
         <v>200</v>
       </c>
       <c r="BA8" s="10">
-        <f t="shared" si="3"/>
+        <f>SUMIF($B$2:$B$1048576,$B8,$AV$2:$AV$1048576)</f>
         <v>764</v>
       </c>
       <c r="BB8" s="10">
-        <f t="shared" si="4"/>
+        <f>SUMIF($B$2:$B$1048576,$B8,$AF$2:$AF$1048576)*60</f>
         <v>871.19380000000194</v>
       </c>
       <c r="BC8" s="10">
-        <f t="shared" ref="BC8" si="13">BB8/AZ8</f>
+        <f t="shared" ref="BC8" si="6">BB8/AZ8</f>
         <v>4.3559690000000097</v>
       </c>
       <c r="BD8" s="10">
-        <f t="shared" si="6"/>
+        <f>SUMIF($B$2:$B$1048576,$B8,$AN$2:$AN$1048576)</f>
         <v>97</v>
       </c>
       <c r="BE8" s="10">
-        <f t="shared" si="7"/>
+        <f>SUMIF($B$2:$B$1048576,$B8,$AO$2:$AO$1048576)</f>
         <v>94</v>
       </c>
       <c r="BF8" s="10">
-        <f t="shared" si="8"/>
+        <f>SUMIF($B$2:$B$1048576,$B8,$AP$2:$AP$1048576)</f>
         <v>0</v>
       </c>
       <c r="BG8" s="10">
-        <f t="shared" si="9"/>
+        <f>SUMIF($B$2:$B$1048576,$B8,$AQ$2:$AQ$1048576)</f>
         <v>0</v>
       </c>
       <c r="BH8" s="22">
-        <f t="shared" ref="BH8" si="14">SUM(BD8,BF8)</f>
+        <f t="shared" ref="BH8" si="7">SUM(BD8,BF8)</f>
         <v>97</v>
       </c>
       <c r="BI8" s="22">
-        <f t="shared" ref="BI8" si="15">SUM(BE8,BG8)</f>
+        <f t="shared" ref="BI8" si="8">SUM(BE8,BG8)</f>
         <v>94</v>
       </c>
     </row>
@@ -22671,50 +22677,50 @@
         <v>92</v>
       </c>
       <c r="AX9" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>'20201113'</v>
       </c>
       <c r="AY9" s="18" t="s">
         <v>221</v>
       </c>
       <c r="AZ9" s="12">
-        <f t="shared" si="2"/>
+        <f>SUMIF($B$2:$B$1048576,$B9,$AE$2:$AE$1048576)</f>
         <v>390</v>
       </c>
       <c r="BA9" s="12">
-        <f t="shared" si="3"/>
+        <f>SUMIF($B$2:$B$1048576,$B9,$AV$2:$AV$1048576)</f>
         <v>1060</v>
       </c>
       <c r="BB9" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIF($B$2:$B$1048576,$B9,$AF$2:$AF$1048576)*60</f>
         <v>2359.8423000000016</v>
       </c>
       <c r="BC9" s="12">
-        <f t="shared" ref="BC9:BC11" si="16">BB9/AZ9</f>
+        <f t="shared" ref="BC9:BC11" si="9">BB9/AZ9</f>
         <v>6.0508776923076963</v>
       </c>
       <c r="BD9" s="12">
-        <f t="shared" si="6"/>
+        <f>SUMIF($B$2:$B$1048576,$B9,$AN$2:$AN$1048576)</f>
         <v>139</v>
       </c>
       <c r="BE9" s="12">
-        <f t="shared" si="7"/>
+        <f>SUMIF($B$2:$B$1048576,$B9,$AO$2:$AO$1048576)</f>
         <v>140</v>
       </c>
       <c r="BF9" s="12">
-        <f t="shared" si="8"/>
+        <f>SUMIF($B$2:$B$1048576,$B9,$AP$2:$AP$1048576)</f>
         <v>0</v>
       </c>
       <c r="BG9" s="12">
-        <f t="shared" si="9"/>
+        <f>SUMIF($B$2:$B$1048576,$B9,$AQ$2:$AQ$1048576)</f>
         <v>0</v>
       </c>
       <c r="BH9" s="1">
-        <f t="shared" ref="BH9:BH11" si="17">SUM(BD9,BF9)</f>
+        <f t="shared" ref="BH9:BH11" si="10">SUM(BD9,BF9)</f>
         <v>139</v>
       </c>
       <c r="BI9" s="1">
-        <f t="shared" ref="BI9:BI11" si="18">SUM(BE9,BG9)</f>
+        <f t="shared" ref="BI9:BI11" si="11">SUM(BE9,BG9)</f>
         <v>140</v>
       </c>
     </row>
@@ -22864,257 +22870,441 @@
         <v>300</v>
       </c>
       <c r="AX10" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>'20201113'</v>
       </c>
       <c r="AY10" s="18" t="s">
         <v>219</v>
       </c>
       <c r="AZ10" s="12">
-        <f t="shared" si="2"/>
+        <f>SUMIF($B$2:$B$1048576,$B10,$AE$2:$AE$1048576)</f>
         <v>390</v>
       </c>
       <c r="BA10" s="12">
-        <f t="shared" si="3"/>
+        <f>SUMIF($B$2:$B$1048576,$B10,$AV$2:$AV$1048576)</f>
         <v>1060</v>
       </c>
       <c r="BB10" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIF($B$2:$B$1048576,$B10,$AF$2:$AF$1048576)*60</f>
         <v>2359.8423000000016</v>
       </c>
       <c r="BC10" s="12">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>6.0508776923076963</v>
       </c>
       <c r="BD10" s="12">
-        <f t="shared" si="6"/>
+        <f>SUMIF($B$2:$B$1048576,$B10,$AN$2:$AN$1048576)</f>
         <v>139</v>
       </c>
       <c r="BE10" s="12">
-        <f t="shared" si="7"/>
+        <f>SUMIF($B$2:$B$1048576,$B10,$AO$2:$AO$1048576)</f>
         <v>140</v>
       </c>
       <c r="BF10" s="12">
-        <f t="shared" si="8"/>
+        <f>SUMIF($B$2:$B$1048576,$B10,$AP$2:$AP$1048576)</f>
         <v>0</v>
       </c>
       <c r="BG10" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B10,$AQ$2:$AQ$1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="BH10" s="1">
+        <f t="shared" si="10"/>
+        <v>139</v>
+      </c>
+      <c r="BI10" s="1">
+        <f t="shared" si="11"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:65" s="22" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" s="22">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="22">
+        <v>4</v>
+      </c>
+      <c r="E11" s="22">
+        <v>0</v>
+      </c>
+      <c r="F11" s="22">
+        <v>3</v>
+      </c>
+      <c r="G11" s="22">
+        <v>2</v>
+      </c>
+      <c r="H11" s="22">
+        <v>1</v>
+      </c>
+      <c r="I11" s="22">
+        <v>1</v>
+      </c>
+      <c r="J11" s="22">
+        <v>0</v>
+      </c>
+      <c r="K11" s="22">
+        <v>3</v>
+      </c>
+      <c r="L11" s="22">
+        <v>2</v>
+      </c>
+      <c r="M11" s="22">
+        <v>0</v>
+      </c>
+      <c r="N11" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="O11" s="22">
+        <v>0</v>
+      </c>
+      <c r="P11" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="Q11" s="22">
+        <v>0</v>
+      </c>
+      <c r="R11" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="S11" s="22">
+        <v>1</v>
+      </c>
+      <c r="T11" s="22">
+        <v>0</v>
+      </c>
+      <c r="U11" s="22">
+        <v>1</v>
+      </c>
+      <c r="V11" s="22">
+        <v>0</v>
+      </c>
+      <c r="W11" s="22">
+        <v>1</v>
+      </c>
+      <c r="X11" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="22">
+        <v>3</v>
+      </c>
+      <c r="Z11" s="22">
+        <v>4</v>
+      </c>
+      <c r="AA11" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="22">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="22">
+        <v>207</v>
+      </c>
+      <c r="AF11" s="22">
+        <v>26.431796666666699</v>
+      </c>
+      <c r="AG11" s="24">
+        <v>0.82142857142857095</v>
+      </c>
+      <c r="AH11" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI11" s="24">
+        <v>0.86607142857142905</v>
+      </c>
+      <c r="AJ11" s="24">
+        <v>0.78571428571428603</v>
+      </c>
+      <c r="AK11" s="22">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="22">
+        <v>97</v>
+      </c>
+      <c r="AM11" s="22">
+        <v>110</v>
+      </c>
+      <c r="AN11" s="22">
+        <v>85</v>
+      </c>
+      <c r="AO11" s="22">
+        <v>85</v>
+      </c>
+      <c r="AP11" s="22">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="22">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS11" s="24">
+        <v>0.82125603864734298</v>
+      </c>
+      <c r="AT11" s="22">
+        <v>340</v>
+      </c>
+      <c r="AU11" s="22">
+        <v>328</v>
+      </c>
+      <c r="AV11" s="22">
+        <v>668</v>
+      </c>
+      <c r="AX11" s="22" t="str">
+        <f t="shared" ref="AX11:AX12" si="12">B11</f>
+        <v>'20201113'</v>
+      </c>
+      <c r="AY11" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ11" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B11,$AE$2:$AE$1048576)</f>
+        <v>390</v>
+      </c>
+      <c r="BA11" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B11,$AV$2:$AV$1048576)</f>
+        <v>1060</v>
+      </c>
+      <c r="BB11" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B11,$AF$2:$AF$1048576)*60</f>
+        <v>2359.8423000000016</v>
+      </c>
+      <c r="BC11" s="10">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BH10" s="1">
-        <f t="shared" si="17"/>
+        <v>6.0508776923076963</v>
+      </c>
+      <c r="BD11" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B11,$AN$2:$AN$1048576)</f>
         <v>139</v>
       </c>
-      <c r="BI10" s="1">
-        <f t="shared" si="18"/>
+      <c r="BE11" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B11,$AO$2:$AO$1048576)</f>
         <v>140</v>
       </c>
-    </row>
-    <row r="11" spans="1:65" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D11" s="1">
-        <v>4</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>3</v>
-      </c>
-      <c r="G11" s="1">
-        <v>2</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
-        <v>3</v>
-      </c>
-      <c r="L11" s="1">
-        <v>2</v>
-      </c>
-      <c r="M11" s="1">
-        <v>0</v>
-      </c>
-      <c r="N11" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="O11" s="1">
-        <v>0</v>
-      </c>
-      <c r="P11" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>0</v>
-      </c>
-      <c r="R11" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="S11" s="1">
-        <v>1</v>
-      </c>
-      <c r="T11" s="1">
-        <v>0</v>
-      </c>
-      <c r="U11" s="1">
-        <v>1</v>
-      </c>
-      <c r="V11" s="1">
-        <v>0</v>
-      </c>
-      <c r="W11" s="1">
-        <v>1</v>
-      </c>
-      <c r="X11" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="1">
-        <v>3</v>
-      </c>
-      <c r="Z11" s="1">
-        <v>4</v>
-      </c>
-      <c r="AA11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="1">
-        <v>207</v>
-      </c>
-      <c r="AF11" s="1">
-        <v>26.431796666666699</v>
-      </c>
-      <c r="AG11" s="8">
-        <v>0.82142857142857095</v>
-      </c>
-      <c r="AH11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI11" s="8">
-        <v>0.86607142857142905</v>
-      </c>
-      <c r="AJ11" s="8">
-        <v>0.78571428571428603</v>
-      </c>
-      <c r="AK11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL11" s="1">
-        <v>97</v>
-      </c>
-      <c r="AM11" s="1">
-        <v>110</v>
-      </c>
-      <c r="AN11" s="1">
-        <v>85</v>
-      </c>
-      <c r="AO11" s="1">
-        <v>85</v>
-      </c>
-      <c r="AP11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS11" s="8">
-        <v>0.82125603864734298</v>
-      </c>
-      <c r="AT11" s="1">
-        <v>340</v>
-      </c>
-      <c r="AU11" s="1">
-        <v>328</v>
-      </c>
-      <c r="AV11" s="1">
-        <v>668</v>
-      </c>
-      <c r="AX11" s="1" t="str">
-        <f t="shared" ref="AX11" si="19">B11</f>
-        <v>'20201113'</v>
-      </c>
-      <c r="AY11" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="AZ11" s="12">
-        <f t="shared" si="2"/>
-        <v>390</v>
-      </c>
-      <c r="BA11" s="12">
-        <f t="shared" si="3"/>
-        <v>1060</v>
-      </c>
-      <c r="BB11" s="12">
-        <f t="shared" si="4"/>
-        <v>2359.8423000000016</v>
-      </c>
-      <c r="BC11" s="12">
-        <f t="shared" si="16"/>
-        <v>6.0508776923076963</v>
-      </c>
-      <c r="BD11" s="12">
-        <f t="shared" si="6"/>
+      <c r="BF11" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B11,$AP$2:$AP$1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="BG11" s="10">
+        <f>SUMIF($B$2:$B$1048576,$B11,$AQ$2:$AQ$1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="BH11" s="22">
+        <f t="shared" si="10"/>
         <v>139</v>
       </c>
-      <c r="BE11" s="12">
-        <f t="shared" si="7"/>
-        <v>140</v>
-      </c>
-      <c r="BF11" s="12">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="BG11" s="12">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BH11" s="1">
-        <f t="shared" si="17"/>
-        <v>139</v>
-      </c>
-      <c r="BI11" s="1">
-        <f t="shared" si="18"/>
+      <c r="BI11" s="22">
+        <f t="shared" si="11"/>
         <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:65" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="AZ12" s="12"/>
-      <c r="BA12" s="12"/>
-      <c r="BB12" s="12"/>
-      <c r="BC12" s="12"/>
-      <c r="BD12" s="12"/>
-      <c r="BE12" s="12"/>
-      <c r="BF12" s="12"/>
-      <c r="BG12" s="12"/>
+      <c r="A12" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>3</v>
+      </c>
+      <c r="L12" s="1">
+        <v>2</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="S12" s="1">
+        <v>1</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
+      <c r="U12" s="1">
+        <v>1</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0</v>
+      </c>
+      <c r="W12" s="1">
+        <v>1</v>
+      </c>
+      <c r="X12" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>318</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>49.866390000000003</v>
+      </c>
+      <c r="AG12" s="8">
+        <v>0.79699248120300803</v>
+      </c>
+      <c r="AH12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI12" s="8">
+        <v>0.76829268292682895</v>
+      </c>
+      <c r="AJ12" s="8">
+        <v>0.84313725490196101</v>
+      </c>
+      <c r="AK12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="1">
+        <v>189</v>
+      </c>
+      <c r="AM12" s="1">
+        <v>129</v>
+      </c>
+      <c r="AN12" s="1">
+        <v>109</v>
+      </c>
+      <c r="AO12" s="1">
+        <v>111</v>
+      </c>
+      <c r="AP12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS12" s="8">
+        <v>0.69182389937106903</v>
+      </c>
+      <c r="AT12" s="1">
+        <v>400</v>
+      </c>
+      <c r="AU12" s="1">
+        <v>440</v>
+      </c>
+      <c r="AV12" s="1">
+        <v>840</v>
+      </c>
+      <c r="AX12" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>'20201116'</v>
+      </c>
+      <c r="AY12" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ12" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B12,$AE$2:$AE$1048576)</f>
+        <v>318</v>
+      </c>
+      <c r="BA12" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B12,$AV$2:$AV$1048576)</f>
+        <v>840</v>
+      </c>
+      <c r="BB12" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B12,$AF$2:$AF$1048576)*60</f>
+        <v>2991.9834000000001</v>
+      </c>
+      <c r="BC12" s="12">
+        <f t="shared" ref="BC12" si="13">BB12/AZ12</f>
+        <v>9.4087528301886802</v>
+      </c>
+      <c r="BD12" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B12,$AN$2:$AN$1048576)</f>
+        <v>109</v>
+      </c>
+      <c r="BE12" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B12,$AO$2:$AO$1048576)</f>
+        <v>111</v>
+      </c>
+      <c r="BF12" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B12,$AP$2:$AP$1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="BG12" s="12">
+        <f>SUMIF($B$2:$B$1048576,$B12,$AQ$2:$AQ$1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="BH12" s="1">
+        <f t="shared" ref="BH12" si="14">SUM(BD12,BF12)</f>
+        <v>109</v>
+      </c>
+      <c r="BI12" s="1">
+        <f t="shared" ref="BI12" si="15">SUM(BE12,BG12)</f>
+        <v>111</v>
+      </c>
     </row>
     <row r="13" spans="1:65" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="AY13" s="18"/>
       <c r="AZ13" s="12"/>
       <c r="BA13" s="12"/>
       <c r="BB13" s="12"/>
@@ -23189,17 +23379,6 @@
       <c r="BE19" s="12"/>
       <c r="BF19" s="12"/>
       <c r="BG19" s="12"/>
-    </row>
-    <row r="20" spans="51:59" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="AY20" s="18"/>
-      <c r="AZ20" s="12"/>
-      <c r="BA20" s="12"/>
-      <c r="BB20" s="12"/>
-      <c r="BC20" s="12"/>
-      <c r="BD20" s="12"/>
-      <c r="BE20" s="12"/>
-      <c r="BF20" s="12"/>
-      <c r="BG20" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25101,8 +25280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>